<commit_message>
# alterado morbidade e intercorrencia
</commit_message>
<xml_diff>
--- a/src/output.xlsx
+++ b/src/output.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="48">
   <si>
     <t>ALOJAMENTO CONJUNTO (444)</t>
   </si>
@@ -32,109 +32,112 @@
     <t>UTIN (214)</t>
   </si>
   <si>
-    <t>False (712)</t>
-  </si>
-  <si>
-    <t>True (128)</t>
-  </si>
-  <si>
-    <t>373</t>
-  </si>
-  <si>
-    <t>71</t>
+    <t>BRANCA (658)</t>
+  </si>
+  <si>
+    <t>NEGRA (25)</t>
+  </si>
+  <si>
+    <t>PARDA (157)</t>
+  </si>
+  <si>
+    <t>358</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>EXTREMO (&lt; 28) (60)</t>
+  </si>
+  <si>
+    <t>GRAVE (28+0 - 31+6) (66)</t>
+  </si>
+  <si>
+    <t>TARDIA (32 - 36+6) (714)</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>563</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>Normal (828)</t>
+  </si>
+  <si>
+    <t>Severamente Deprimido (12)</t>
+  </si>
+  <si>
+    <t>648</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>155</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>145</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>184</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>EXTREMO (&lt; 28) (60)</t>
-  </si>
-  <si>
-    <t>GRAVE (28+0 - 31+6) (66)</t>
-  </si>
-  <si>
-    <t>TARDIA (32 - 36+6) (714)</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>59</t>
-  </si>
-  <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>114</t>
-  </si>
-  <si>
-    <t>Moderadamente Deprimido (84)</t>
-  </si>
-  <si>
-    <t>Normal (700)</t>
-  </si>
-  <si>
-    <t>Severamente Deprimido (56)</t>
-  </si>
-  <si>
-    <t>73</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>595</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>44</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Moderadamente Deprimido (24)</t>
-  </si>
-  <si>
-    <t>Normal (804)</t>
-  </si>
-  <si>
-    <t>Severamente Deprimido (12)</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>678</t>
-  </si>
-  <si>
-    <t>126</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>Normal (838)</t>
+  </si>
+  <si>
+    <t>Severamente Deprimido (2)</t>
+  </si>
+  <si>
+    <t>657</t>
+  </si>
+  <si>
+    <t>156</t>
   </si>
   <si>
     <t>Aumentou (708)</t>
@@ -146,13 +149,19 @@
     <t>Permaneceu Igual (130)</t>
   </si>
   <si>
-    <t>603</t>
-  </si>
-  <si>
-    <t>107</t>
-  </si>
-  <si>
-    <t>23</t>
+    <t>555</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
 </sst>
 </file>
@@ -510,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -535,16 +544,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -552,16 +561,33 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -571,7 +597,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -579,13 +605,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -593,13 +619,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -607,13 +633,27 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -623,7 +663,115 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -631,13 +779,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -645,13 +793,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -659,117 +807,27 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>